<commit_message>
Mode updates to link prediction model code and mpxv virion records.
</commit_message>
<xml_diff>
--- a/Tseng2022/PoxHost_InteractionMatrices.xlsx
+++ b/Tseng2022/PoxHost_InteractionMatrices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailwsu-my.sharepoint.com/personal/katie_tseng_wsu_edu/Documents/Fernandez Lab/Projects (Active)/OPV Host Prediction/GitHub/PoxHost/Tseng2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="728" documentId="8_{CECB39CC-D9D5-0C45-9DA2-CA875FC6CA1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F4FABC3C-FF3C-B946-8402-7AE8C028F2E8}"/>
+  <xr:revisionPtr revIDLastSave="737" documentId="8_{CECB39CC-D9D5-0C45-9DA2-CA875FC6CA1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ABE1834F-77E3-CC45-BF6B-2C6F613A2148}"/>
   <bookViews>
-    <workbookView xWindow="29860" yWindow="500" windowWidth="27480" windowHeight="17500" activeTab="1" xr2:uid="{AEA15567-D228-154F-A7A4-0A59ECBFD0F2}"/>
+    <workbookView xWindow="30760" yWindow="2220" windowWidth="35720" windowHeight="18260" activeTab="1" xr2:uid="{AEA15567-D228-154F-A7A4-0A59ECBFD0F2}"/>
   </bookViews>
   <sheets>
     <sheet name="HostVirus_interactions" sheetId="1" r:id="rId1"/>
@@ -1596,27 +1596,6 @@
     <t>Common squirrel monkey; strain unknown based on reference texts; ILL request pending for Fenner et al. 1989 and von Magnus et al. 1959; Peters 1966, Fenner 1994 and España 1971 provided no add'l information</t>
   </si>
   <si>
-    <t>Rhesus macaque; strain unknown based on reference texts; ILL request pending for Fenner et al. 1989 and von Magnus et al. 1959; Peters 1966, Fenner 1994 and España 1971 provided no add'l information</t>
-  </si>
-  <si>
-    <t>Crab-eating macaque; strain unknown based on reference texts; ILL request pending for Fenner et al. 1989 and von Magnus et al. 1959; Peters 1966, Fenner 1994 and España 1971 provided no add'l information</t>
-  </si>
-  <si>
-    <t>Lar gibbon; strain unknown based on reference texts; ILL request pending for Fenner et al. 1989 and von Magnus et al. 1959; Peters 1966, Fenner 1994 and España 1971 provided no add'l information</t>
-  </si>
-  <si>
-    <t>Human; strain unknown based on reference texts; ILL request pending for Fenner et al. 1989 and von Magnus et al. 1959; Peters 1966, Fenner 1994 and España 1971 provided no add'l information</t>
-  </si>
-  <si>
-    <t>Thomas's rope squirrel; strain unknown based on reference texts; ILL request pending for Fenner et al. 1989 and von Magnus et al. 1959; Peters 1966, Fenner 1994 and España 1971 provided no add'l information</t>
-  </si>
-  <si>
-    <t>Prairie dog; strain unknown based on reference texts; ILL request pending for Fenner et al. 1989 and von Magnus et al. 1959; Peters 1966, Fenner 1994 and España 1971 provided no add'l information</t>
-  </si>
-  <si>
-    <t>Common marmoset; strain unknown based on reference texts; ILL request pending for Fenner et al. 1989 and von Magnus et al. 1959; Peters 1966, Fenner 1994 and España 1971 provided no add'l information</t>
-  </si>
-  <si>
     <t>Thomas's rope squirrel isolation-positive for MPXV in Khodakevich et al. 1986 Lancet (surveyed in Northern Zaire within 40km of Yambuku, Bumba zone)</t>
   </si>
   <si>
@@ -1714,6 +1693,27 @@
   </si>
   <si>
     <t>AF375094.1, AF375095.1, AF375096.1, AF375097.1, AF375098.1, AF375099.1, AF375100.1, AF375101.1, AF375102.1, AF375103.1, AF375104.1</t>
+  </si>
+  <si>
+    <t>Common marmoset; strain unknown based on reference texts; ILL request pending for Fenner et al. 1989;  von Magnus 1959, Peters 1966, Fenner 1994 and España 1971 provided no add'l information</t>
+  </si>
+  <si>
+    <t>Prairie dog; strain unknown based on reference texts; ILL request pending for Fenner et al. 1989; von Magnus 1959, Peters 1966, Fenner 1994 and España 1971 provided no add'l information</t>
+  </si>
+  <si>
+    <t>Thomas's rope squirrel; strain unknown based on reference texts; ILL request pending for Fenner et al. 1989; von Magnus 1959, Peters 1966, Fenner 1994 and España 1971 provided no add'l information</t>
+  </si>
+  <si>
+    <t>Human; strain unknown based on reference texts; ILL request pending for Fenner et al. 1989; von Magnus 1959, Peters 1966, Fenner 1994 and España 1971 provided no add'l information</t>
+  </si>
+  <si>
+    <t>Lar gibbon; strain unknown based on reference texts; ILL request pending for Fenner et al. 1989; von Magnus 1959, Peters 1966, Fenner 1994 and España 1971 provided no add'l information</t>
+  </si>
+  <si>
+    <t>Crab-eating macaque; strain unknown based on reference texts; ILL request pending for Fenner et al. 1989; von Magnus 1959 isolated MPXV from macaca spp. (did not specify fascicularis or rhesus); Peters 1966, Fenner 1994 and España 1971 provided no add'l information</t>
+  </si>
+  <si>
+    <t>Rhesus macaque; strain unknown based on reference texts; ILL request pending for Fenner et al. 1989; von Magnus 1959 isolated MPXV from macaca spp. (did not specify fascicularis or rhesus); Peters 1966, Fenner 1994 and España 1971 provided no add'l information</t>
   </si>
 </sst>
 </file>
@@ -2789,20 +2789,25 @@
   <dimension ref="A1:AL190"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E35" sqref="E35"/>
+      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AJ163" sqref="AJ163"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="18.83203125" customWidth="1"/>
-    <col min="3" max="7" width="10.83203125" customWidth="1"/>
-    <col min="8" max="8" width="7.33203125" customWidth="1"/>
-    <col min="11" max="12" width="10.83203125" customWidth="1"/>
-    <col min="14" max="18" width="10.83203125" customWidth="1"/>
+    <col min="3" max="3" width="10.83203125" customWidth="1"/>
+    <col min="4" max="7" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="7.33203125" hidden="1" customWidth="1"/>
+    <col min="9" max="10" width="0" hidden="1" customWidth="1"/>
+    <col min="11" max="12" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="0" hidden="1" customWidth="1"/>
+    <col min="14" max="18" width="10.83203125" hidden="1" customWidth="1"/>
     <col min="19" max="19" width="1.83203125" customWidth="1"/>
     <col min="21" max="21" width="10.83203125" customWidth="1"/>
-    <col min="25" max="34" width="10.83203125" customWidth="1"/>
+    <col min="25" max="26" width="10.83203125" customWidth="1"/>
+    <col min="27" max="32" width="10.83203125" hidden="1" customWidth="1"/>
+    <col min="33" max="34" width="10.83203125" customWidth="1"/>
     <col min="36" max="36" width="12.1640625" customWidth="1"/>
     <col min="37" max="37" width="22" customWidth="1"/>
     <col min="38" max="38" width="29.1640625" customWidth="1"/>
@@ -11183,7 +11188,7 @@
         <v>42</v>
       </c>
       <c r="AI76" t="s">
-        <v>557</v>
+        <v>550</v>
       </c>
       <c r="AJ76" t="s">
         <v>470</v>
@@ -11227,7 +11232,7 @@
         <v>357</v>
       </c>
       <c r="M77" t="s">
-        <v>556</v>
+        <v>549</v>
       </c>
       <c r="N77" t="s">
         <v>356</v>
@@ -11293,7 +11298,7 @@
         <v>42</v>
       </c>
       <c r="AI77" t="s">
-        <v>555</v>
+        <v>548</v>
       </c>
       <c r="AJ77" t="s">
         <v>470</v>
@@ -11447,7 +11452,7 @@
         <v>357</v>
       </c>
       <c r="M79" t="s">
-        <v>554</v>
+        <v>547</v>
       </c>
       <c r="N79" t="s">
         <v>356</v>
@@ -11513,7 +11518,7 @@
         <v>42</v>
       </c>
       <c r="AI79" t="s">
-        <v>553</v>
+        <v>546</v>
       </c>
       <c r="AJ79" t="s">
         <v>470</v>
@@ -11623,7 +11628,7 @@
         <v>42</v>
       </c>
       <c r="AI80" t="s">
-        <v>552</v>
+        <v>545</v>
       </c>
       <c r="AJ80" t="s">
         <v>470</v>
@@ -11843,7 +11848,7 @@
         <v>42</v>
       </c>
       <c r="AI82" t="s">
-        <v>551</v>
+        <v>544</v>
       </c>
       <c r="AJ82" t="s">
         <v>470</v>
@@ -11953,7 +11958,7 @@
         <v>42</v>
       </c>
       <c r="AI83" t="s">
-        <v>550</v>
+        <v>543</v>
       </c>
       <c r="AJ83" t="s">
         <v>470</v>
@@ -12063,7 +12068,7 @@
         <v>42</v>
       </c>
       <c r="AI84" t="s">
-        <v>549</v>
+        <v>542</v>
       </c>
       <c r="AJ84" t="s">
         <v>470</v>
@@ -12173,7 +12178,7 @@
         <v>42</v>
       </c>
       <c r="AI85" t="s">
-        <v>548</v>
+        <v>541</v>
       </c>
       <c r="AJ85" t="s">
         <v>470</v>
@@ -12283,7 +12288,7 @@
         <v>42</v>
       </c>
       <c r="AI86" t="s">
-        <v>547</v>
+        <v>540</v>
       </c>
       <c r="AJ86" t="s">
         <v>470</v>
@@ -13273,7 +13278,7 @@
         <v>42</v>
       </c>
       <c r="AI95" t="s">
-        <v>546</v>
+        <v>539</v>
       </c>
       <c r="AJ95" t="s">
         <v>470</v>
@@ -13383,7 +13388,7 @@
         <v>42</v>
       </c>
       <c r="AI96" t="s">
-        <v>545</v>
+        <v>538</v>
       </c>
       <c r="AJ96" t="s">
         <v>470</v>
@@ -13493,7 +13498,7 @@
         <v>42</v>
       </c>
       <c r="AI97" t="s">
-        <v>544</v>
+        <v>537</v>
       </c>
       <c r="AJ97" t="s">
         <v>470</v>
@@ -14153,7 +14158,7 @@
         <v>42</v>
       </c>
       <c r="AI103" t="s">
-        <v>543</v>
+        <v>536</v>
       </c>
       <c r="AJ103" t="s">
         <v>470</v>
@@ -15077,7 +15082,7 @@
         <v>357</v>
       </c>
       <c r="M112" t="s">
-        <v>542</v>
+        <v>535</v>
       </c>
       <c r="N112" t="s">
         <v>356</v>
@@ -15143,7 +15148,7 @@
         <v>42</v>
       </c>
       <c r="AI112" t="s">
-        <v>541</v>
+        <v>534</v>
       </c>
       <c r="AJ112" t="s">
         <v>470</v>
@@ -15253,7 +15258,7 @@
         <v>42</v>
       </c>
       <c r="AI113" t="s">
-        <v>540</v>
+        <v>533</v>
       </c>
       <c r="AJ113" t="s">
         <v>470</v>
@@ -15363,7 +15368,7 @@
         <v>42</v>
       </c>
       <c r="AI114" t="s">
-        <v>539</v>
+        <v>532</v>
       </c>
       <c r="AJ114" t="s">
         <v>470</v>
@@ -15473,7 +15478,7 @@
         <v>42</v>
       </c>
       <c r="AI115" t="s">
-        <v>538</v>
+        <v>531</v>
       </c>
       <c r="AJ115" t="s">
         <v>470</v>
@@ -15803,7 +15808,7 @@
         <v>42</v>
       </c>
       <c r="AI118" t="s">
-        <v>537</v>
+        <v>530</v>
       </c>
       <c r="AJ118" t="s">
         <v>470</v>
@@ -15913,7 +15918,7 @@
         <v>42</v>
       </c>
       <c r="AI119" t="s">
-        <v>536</v>
+        <v>529</v>
       </c>
       <c r="AJ119" t="s">
         <v>470</v>
@@ -16023,7 +16028,7 @@
         <v>42</v>
       </c>
       <c r="AI120" t="s">
-        <v>535</v>
+        <v>528</v>
       </c>
       <c r="AJ120" t="s">
         <v>470</v>
@@ -18113,7 +18118,7 @@
         <v>42</v>
       </c>
       <c r="AI139" t="s">
-        <v>534</v>
+        <v>527</v>
       </c>
       <c r="AJ139" t="s">
         <v>470</v>
@@ -19543,7 +19548,7 @@
         <v>42</v>
       </c>
       <c r="AI152" t="s">
-        <v>533</v>
+        <v>526</v>
       </c>
       <c r="AJ152" t="s">
         <v>470</v>
@@ -19766,10 +19771,10 @@
         <v>42</v>
       </c>
       <c r="AJ154" t="s">
-        <v>527</v>
+        <v>520</v>
       </c>
       <c r="AL154" t="s">
-        <v>532</v>
+        <v>525</v>
       </c>
     </row>
     <row r="155" spans="1:38" x14ac:dyDescent="0.2">
@@ -19879,10 +19884,10 @@
         <v>42</v>
       </c>
       <c r="AJ155" t="s">
-        <v>527</v>
+        <v>520</v>
       </c>
       <c r="AL155" t="s">
-        <v>531</v>
+        <v>524</v>
       </c>
     </row>
     <row r="156" spans="1:38" x14ac:dyDescent="0.2">
@@ -19992,10 +19997,10 @@
         <v>42</v>
       </c>
       <c r="AJ156" t="s">
-        <v>527</v>
+        <v>520</v>
       </c>
       <c r="AL156" t="s">
-        <v>530</v>
+        <v>523</v>
       </c>
     </row>
     <row r="157" spans="1:38" x14ac:dyDescent="0.2">
@@ -20105,10 +20110,10 @@
         <v>42</v>
       </c>
       <c r="AJ157" t="s">
-        <v>527</v>
+        <v>520</v>
       </c>
       <c r="AL157" t="s">
-        <v>529</v>
+        <v>522</v>
       </c>
     </row>
     <row r="158" spans="1:38" x14ac:dyDescent="0.2">
@@ -20218,10 +20223,10 @@
         <v>42</v>
       </c>
       <c r="AJ158" t="s">
-        <v>527</v>
+        <v>520</v>
       </c>
       <c r="AL158" t="s">
-        <v>528</v>
+        <v>521</v>
       </c>
     </row>
     <row r="159" spans="1:38" x14ac:dyDescent="0.2">
@@ -20331,10 +20336,10 @@
         <v>42</v>
       </c>
       <c r="AJ159" t="s">
-        <v>527</v>
+        <v>520</v>
       </c>
       <c r="AL159" s="16" t="s">
-        <v>526</v>
+        <v>519</v>
       </c>
     </row>
     <row r="160" spans="1:38" x14ac:dyDescent="0.2">
@@ -20447,7 +20452,7 @@
         <v>508</v>
       </c>
       <c r="AL160" t="s">
-        <v>525</v>
+        <v>518</v>
       </c>
     </row>
     <row r="161" spans="1:38" x14ac:dyDescent="0.2">
@@ -20557,7 +20562,7 @@
         <v>42</v>
       </c>
       <c r="AL161" t="s">
-        <v>524</v>
+        <v>551</v>
       </c>
     </row>
     <row r="162" spans="1:38" x14ac:dyDescent="0.2">
@@ -20667,7 +20672,7 @@
         <v>42</v>
       </c>
       <c r="AL162" t="s">
-        <v>523</v>
+        <v>552</v>
       </c>
     </row>
     <row r="163" spans="1:38" x14ac:dyDescent="0.2">
@@ -20777,7 +20782,7 @@
         <v>42</v>
       </c>
       <c r="AL163" t="s">
-        <v>522</v>
+        <v>553</v>
       </c>
     </row>
     <row r="164" spans="1:38" x14ac:dyDescent="0.2">
@@ -20887,7 +20892,7 @@
         <v>42</v>
       </c>
       <c r="AL164" t="s">
-        <v>521</v>
+        <v>554</v>
       </c>
     </row>
     <row r="165" spans="1:38" x14ac:dyDescent="0.2">
@@ -20997,7 +21002,7 @@
         <v>42</v>
       </c>
       <c r="AL165" t="s">
-        <v>520</v>
+        <v>555</v>
       </c>
     </row>
     <row r="166" spans="1:38" x14ac:dyDescent="0.2">
@@ -21107,7 +21112,7 @@
         <v>42</v>
       </c>
       <c r="AL166" t="s">
-        <v>519</v>
+        <v>556</v>
       </c>
     </row>
     <row r="167" spans="1:38" x14ac:dyDescent="0.2">
@@ -21217,7 +21222,7 @@
         <v>42</v>
       </c>
       <c r="AL167" t="s">
-        <v>518</v>
+        <v>557</v>
       </c>
     </row>
     <row r="168" spans="1:38" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
updated merging of viralTraits code
</commit_message>
<xml_diff>
--- a/Tseng2022/PoxHost_InteractionMatrices.xlsx
+++ b/Tseng2022/PoxHost_InteractionMatrices.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://emailwsu-my.sharepoint.com/personal/katie_tseng_wsu_edu/Documents/Fernandez Lab/Projects (Active)/OPV Host Prediction/GitHub/PoxHost/Tseng2022/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="737" documentId="8_{CECB39CC-D9D5-0C45-9DA2-CA875FC6CA1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{ABE1834F-77E3-CC45-BF6B-2C6F613A2148}"/>
+  <xr:revisionPtr revIDLastSave="741" documentId="8_{CECB39CC-D9D5-0C45-9DA2-CA875FC6CA1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{08AA191F-6E3C-6F4F-96A8-5F70BF19B5BB}"/>
   <bookViews>
-    <workbookView xWindow="30760" yWindow="2220" windowWidth="35720" windowHeight="18260" activeTab="1" xr2:uid="{AEA15567-D228-154F-A7A4-0A59ECBFD0F2}"/>
+    <workbookView xWindow="29000" yWindow="500" windowWidth="35720" windowHeight="18260" activeTab="1" xr2:uid="{AEA15567-D228-154F-A7A4-0A59ECBFD0F2}"/>
   </bookViews>
   <sheets>
     <sheet name="HostVirus_interactions" sheetId="1" r:id="rId1"/>
@@ -2786,11 +2786,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7C95825-1A49-044C-8BE1-98126CDF7BB4}">
-  <dimension ref="A1:AL190"/>
+  <dimension ref="A1:AL383"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A152" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AJ163" sqref="AJ163"/>
+      <pane ySplit="1" topLeftCell="A166" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B200" sqref="B200:B383"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23419,6 +23419,558 @@
       <c r="AL190" s="12" t="s">
         <v>480</v>
       </c>
+    </row>
+    <row r="200" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B200" s="5"/>
+    </row>
+    <row r="201" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B201" s="5"/>
+    </row>
+    <row r="202" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B202" s="5"/>
+    </row>
+    <row r="203" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B203" s="5"/>
+    </row>
+    <row r="204" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B204" s="5"/>
+    </row>
+    <row r="205" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B205" s="5"/>
+    </row>
+    <row r="206" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B206" s="5"/>
+    </row>
+    <row r="207" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B207" s="5"/>
+    </row>
+    <row r="208" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B208" s="5"/>
+    </row>
+    <row r="209" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B209" s="5"/>
+    </row>
+    <row r="210" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B210" s="5"/>
+    </row>
+    <row r="211" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B211" s="5"/>
+    </row>
+    <row r="212" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B212" s="5"/>
+    </row>
+    <row r="213" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B213" s="5"/>
+    </row>
+    <row r="214" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B214" s="5"/>
+    </row>
+    <row r="215" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B215" s="5"/>
+    </row>
+    <row r="216" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B216" s="5"/>
+    </row>
+    <row r="217" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B217" s="5"/>
+    </row>
+    <row r="218" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B218" s="5"/>
+    </row>
+    <row r="219" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B219" s="5"/>
+    </row>
+    <row r="220" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B220" s="5"/>
+    </row>
+    <row r="221" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B221" s="5"/>
+    </row>
+    <row r="222" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B222" s="5"/>
+    </row>
+    <row r="223" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B223" s="5"/>
+    </row>
+    <row r="224" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B224" s="5"/>
+    </row>
+    <row r="225" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B225" s="5"/>
+    </row>
+    <row r="226" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B226" s="5"/>
+    </row>
+    <row r="227" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B227" s="5"/>
+    </row>
+    <row r="228" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B228" s="5"/>
+    </row>
+    <row r="229" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B229" s="5"/>
+    </row>
+    <row r="230" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B230" s="5"/>
+    </row>
+    <row r="231" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B231" s="5"/>
+    </row>
+    <row r="232" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B232" s="5"/>
+    </row>
+    <row r="233" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B233" s="5"/>
+    </row>
+    <row r="234" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B234" s="5"/>
+    </row>
+    <row r="235" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B235" s="5"/>
+    </row>
+    <row r="236" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B236" s="5"/>
+    </row>
+    <row r="237" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B237" s="5"/>
+    </row>
+    <row r="238" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B238" s="5"/>
+    </row>
+    <row r="239" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B239" s="5"/>
+    </row>
+    <row r="240" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B240" s="5"/>
+    </row>
+    <row r="241" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B241" s="5"/>
+    </row>
+    <row r="242" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B242" s="5"/>
+    </row>
+    <row r="243" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B243" s="5"/>
+    </row>
+    <row r="244" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B244" s="5"/>
+    </row>
+    <row r="245" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B245" s="5"/>
+    </row>
+    <row r="246" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B246" s="5"/>
+    </row>
+    <row r="247" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B247" s="5"/>
+    </row>
+    <row r="248" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B248" s="5"/>
+    </row>
+    <row r="249" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B249" s="5"/>
+    </row>
+    <row r="250" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B250" s="5"/>
+    </row>
+    <row r="251" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B251" s="5"/>
+    </row>
+    <row r="252" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B252" s="5"/>
+    </row>
+    <row r="253" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B253" s="5"/>
+    </row>
+    <row r="254" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B254" s="5"/>
+    </row>
+    <row r="255" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B255" s="5"/>
+    </row>
+    <row r="256" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B256" s="5"/>
+    </row>
+    <row r="257" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B257" s="5"/>
+    </row>
+    <row r="258" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B258" s="5"/>
+    </row>
+    <row r="259" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B259" s="5"/>
+    </row>
+    <row r="260" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B260" s="5"/>
+    </row>
+    <row r="261" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B261" s="5"/>
+    </row>
+    <row r="262" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B262" s="5"/>
+    </row>
+    <row r="263" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B263" s="5"/>
+    </row>
+    <row r="264" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B264" s="5"/>
+    </row>
+    <row r="265" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B265" s="5"/>
+    </row>
+    <row r="266" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B266" s="5"/>
+    </row>
+    <row r="267" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B267" s="5"/>
+    </row>
+    <row r="268" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B268" s="5"/>
+    </row>
+    <row r="269" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B269" s="5"/>
+    </row>
+    <row r="270" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B270" s="5"/>
+    </row>
+    <row r="271" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B271" s="5"/>
+    </row>
+    <row r="272" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B272" s="5"/>
+    </row>
+    <row r="273" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B273" s="5"/>
+    </row>
+    <row r="274" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B274" s="5"/>
+    </row>
+    <row r="275" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B275" s="5"/>
+    </row>
+    <row r="276" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B276" s="5"/>
+    </row>
+    <row r="277" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B277" s="5"/>
+    </row>
+    <row r="278" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B278" s="5"/>
+    </row>
+    <row r="279" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B279" s="5"/>
+    </row>
+    <row r="280" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B280" s="5"/>
+    </row>
+    <row r="281" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B281" s="5"/>
+    </row>
+    <row r="282" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B282" s="5"/>
+    </row>
+    <row r="283" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B283" s="5"/>
+    </row>
+    <row r="284" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B284" s="5"/>
+    </row>
+    <row r="285" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B285" s="5"/>
+    </row>
+    <row r="286" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B286" s="5"/>
+    </row>
+    <row r="287" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B287" s="5"/>
+    </row>
+    <row r="288" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B288" s="5"/>
+    </row>
+    <row r="289" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B289" s="5"/>
+    </row>
+    <row r="290" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B290" s="5"/>
+    </row>
+    <row r="291" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B291" s="5"/>
+    </row>
+    <row r="292" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B292" s="5"/>
+    </row>
+    <row r="293" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B293" s="5"/>
+    </row>
+    <row r="294" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B294" s="5"/>
+    </row>
+    <row r="295" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B295" s="5"/>
+    </row>
+    <row r="296" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B296" s="5"/>
+    </row>
+    <row r="297" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B297" s="5"/>
+    </row>
+    <row r="298" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B298" s="5"/>
+    </row>
+    <row r="299" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B299" s="5"/>
+    </row>
+    <row r="300" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B300" s="5"/>
+    </row>
+    <row r="301" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B301" s="5"/>
+    </row>
+    <row r="302" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B302" s="5"/>
+    </row>
+    <row r="303" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B303" s="5"/>
+    </row>
+    <row r="304" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B304" s="5"/>
+    </row>
+    <row r="305" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B305" s="5"/>
+    </row>
+    <row r="306" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B306" s="5"/>
+    </row>
+    <row r="307" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B307" s="5"/>
+    </row>
+    <row r="308" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B308" s="5"/>
+    </row>
+    <row r="309" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B309" s="5"/>
+    </row>
+    <row r="310" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B310" s="5"/>
+    </row>
+    <row r="311" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B311" s="5"/>
+    </row>
+    <row r="312" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B312" s="5"/>
+    </row>
+    <row r="313" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B313" s="5"/>
+    </row>
+    <row r="314" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B314" s="5"/>
+    </row>
+    <row r="315" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B315" s="5"/>
+    </row>
+    <row r="316" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B316" s="5"/>
+    </row>
+    <row r="317" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B317" s="5"/>
+    </row>
+    <row r="318" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B318" s="5"/>
+    </row>
+    <row r="319" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B319" s="5"/>
+    </row>
+    <row r="320" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B320" s="5"/>
+    </row>
+    <row r="321" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B321" s="5"/>
+    </row>
+    <row r="322" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B322" s="5"/>
+    </row>
+    <row r="323" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B323" s="5"/>
+    </row>
+    <row r="324" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B324" s="5"/>
+    </row>
+    <row r="325" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B325" s="5"/>
+    </row>
+    <row r="326" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B326" s="5"/>
+    </row>
+    <row r="327" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B327" s="5"/>
+    </row>
+    <row r="328" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B328" s="5"/>
+    </row>
+    <row r="329" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B329" s="5"/>
+    </row>
+    <row r="330" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B330" s="5"/>
+    </row>
+    <row r="331" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B331" s="5"/>
+    </row>
+    <row r="332" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B332" s="5"/>
+    </row>
+    <row r="333" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B333" s="5"/>
+    </row>
+    <row r="334" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B334" s="5"/>
+    </row>
+    <row r="335" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B335" s="5"/>
+    </row>
+    <row r="336" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B336" s="5"/>
+    </row>
+    <row r="337" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B337" s="5"/>
+    </row>
+    <row r="338" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B338" s="5"/>
+    </row>
+    <row r="339" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B339" s="5"/>
+    </row>
+    <row r="340" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B340" s="5"/>
+    </row>
+    <row r="341" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B341" s="5"/>
+    </row>
+    <row r="342" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B342" s="5"/>
+    </row>
+    <row r="343" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B343" s="5"/>
+    </row>
+    <row r="344" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B344" s="5"/>
+    </row>
+    <row r="345" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B345" s="5"/>
+    </row>
+    <row r="346" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B346" s="5"/>
+    </row>
+    <row r="347" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B347" s="5"/>
+    </row>
+    <row r="348" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B348" s="5"/>
+    </row>
+    <row r="349" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B349" s="5"/>
+    </row>
+    <row r="350" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B350" s="5"/>
+    </row>
+    <row r="351" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B351" s="5"/>
+    </row>
+    <row r="352" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B352" s="5"/>
+    </row>
+    <row r="353" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B353" s="5"/>
+    </row>
+    <row r="354" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B354" s="5"/>
+    </row>
+    <row r="355" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B355" s="5"/>
+    </row>
+    <row r="356" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B356" s="5"/>
+    </row>
+    <row r="357" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B357" s="5"/>
+    </row>
+    <row r="358" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B358" s="5"/>
+    </row>
+    <row r="359" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B359" s="5"/>
+    </row>
+    <row r="360" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B360" s="5"/>
+    </row>
+    <row r="361" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B361" s="5"/>
+    </row>
+    <row r="362" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B362" s="5"/>
+    </row>
+    <row r="363" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B363" s="5"/>
+    </row>
+    <row r="364" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B364" s="5"/>
+    </row>
+    <row r="365" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B365" s="5"/>
+    </row>
+    <row r="366" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B366" s="5"/>
+    </row>
+    <row r="367" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B367" s="5"/>
+    </row>
+    <row r="368" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B368" s="5"/>
+    </row>
+    <row r="369" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B369" s="5"/>
+    </row>
+    <row r="370" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B370" s="5"/>
+    </row>
+    <row r="371" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B371" s="5"/>
+    </row>
+    <row r="372" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B372" s="5"/>
+    </row>
+    <row r="373" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B373" s="5"/>
+    </row>
+    <row r="374" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B374" s="5"/>
+    </row>
+    <row r="375" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B375" s="5"/>
+    </row>
+    <row r="376" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B376" s="5"/>
+    </row>
+    <row r="377" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B377" s="5"/>
+    </row>
+    <row r="378" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B378" s="5"/>
+    </row>
+    <row r="379" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B379" s="5"/>
+    </row>
+    <row r="380" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B380" s="5"/>
+    </row>
+    <row r="381" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B381" s="5"/>
+    </row>
+    <row r="382" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B382" s="5"/>
+    </row>
+    <row r="383" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B383" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>